<commit_message>
Grid NN: mid grid training update, more training of mid grid trial 2
Results: showing some shape of a HR diagram, but conclusion is it requires more training, passing onto Guy as training job #3
</commit_message>
<xml_diff>
--- a/Hin's_files/NNgrids_notes.xlsx
+++ b/Hin's_files/NNgrids_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\UoB physics stuff\year 4\FYP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0453224-10AF-42C8-8935-8DD58E77D86D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414C4767-872C-473D-A9F6-C0FDB2CFC42E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{27E1F3F0-F425-4B4B-8745-3E9458FE7065}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="43">
   <si>
     <t>details</t>
   </si>
@@ -151,6 +151,15 @@
   </si>
   <si>
     <t>L shape of HR diagram is present in predicted, requires more training</t>
+  </si>
+  <si>
+    <t>more training of 2</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>main sequence bit now looks better than 2, but still requires more training, sending to Guy</t>
   </si>
 </sst>
 </file>
@@ -514,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7973A843-EDF6-4158-B183-D0716657A8E3}">
-  <dimension ref="A1:O28"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1114,42 +1123,83 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27">
-        <v>4</v>
-      </c>
-      <c r="D27">
-        <v>32</v>
-      </c>
-      <c r="E27">
-        <v>1E-4</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-      <c r="H27">
-        <v>4310530</v>
-      </c>
-      <c r="I27">
-        <v>2000</v>
-      </c>
-      <c r="J27">
-        <v>5.0880000000000002E-2</v>
-      </c>
-      <c r="K27">
-        <v>5.5100000000000003E-2</v>
-      </c>
-      <c r="L27" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2</v>
+      </c>
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28">
+        <v>32</v>
+      </c>
+      <c r="E28">
+        <v>1E-4</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>4310530</v>
+      </c>
+      <c r="I28">
+        <v>2000</v>
+      </c>
+      <c r="J28">
+        <v>5.0880000000000002E-2</v>
+      </c>
+      <c r="K28">
+        <v>5.5100000000000003E-2</v>
+      </c>
+      <c r="L28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29">
+        <v>32</v>
+      </c>
+      <c r="E29">
+        <v>1E-4</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>4310530</v>
+      </c>
+      <c r="I29">
+        <v>12000</v>
+      </c>
+      <c r="J29">
+        <v>4.6289999999999998E-2</v>
+      </c>
+      <c r="K29">
+        <v>5.21E-2</v>
+      </c>
+      <c r="L29" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Grid NN: results after small_grid_model.h5 is trained by Guy
</commit_message>
<xml_diff>
--- a/Hin's_files/NNgrids_notes.xlsx
+++ b/Hin's_files/NNgrids_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\UoB physics stuff\year 4\FYP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414C4767-872C-473D-A9F6-C0FDB2CFC42E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A2B455-7ADE-461B-B79E-4074FAE00403}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{27E1F3F0-F425-4B4B-8745-3E9458FE7065}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="45">
   <si>
     <t>details</t>
   </si>
@@ -160,6 +160,12 @@
   </si>
   <si>
     <t>main sequence bit now looks better than 2, but still requires more training, sending to Guy</t>
+  </si>
+  <si>
+    <t>more training of 7</t>
+  </si>
+  <si>
+    <t>quite close to the real shape, even got the 2 bumps near MS, but jaggered at points. The history plot showed that it is starting to overfit (evaluation loss goes up after ~ 75000 epochs)</t>
   </si>
 </sst>
 </file>
@@ -525,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7973A843-EDF6-4158-B183-D0716657A8E3}">
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,6 +1078,44 @@
         <v>33</v>
       </c>
     </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>10</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <v>32</v>
+      </c>
+      <c r="E22">
+        <v>1E-4</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>9211</v>
+      </c>
+      <c r="I22">
+        <v>250000</v>
+      </c>
+      <c r="J22">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="K22">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="L22" t="s">
+        <v>44</v>
+      </c>
+    </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Grid NN: notes spreadsheet with updates for numbers on trials 11-17
</commit_message>
<xml_diff>
--- a/Hin's_files/NNgrids_notes.xlsx
+++ b/Hin's_files/NNgrids_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\UoB physics stuff\year 4\FYP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A2B455-7ADE-461B-B79E-4074FAE00403}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0548801-4359-45CA-824F-341F4D28A0AF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{27E1F3F0-F425-4B4B-8745-3E9458FE7065}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="62">
   <si>
     <t>details</t>
   </si>
@@ -166,6 +166,57 @@
   </si>
   <si>
     <t>quite close to the real shape, even got the 2 bumps near MS, but jaggered at points. The history plot showed that it is starting to overfit (evaluation loss goes up after ~ 75000 epochs)</t>
+  </si>
+  <si>
+    <t>increasing beta 1</t>
+  </si>
+  <si>
+    <t>rather good performance in just 10k epochs compared to others, training more</t>
+  </si>
+  <si>
+    <t>more training of 11</t>
+  </si>
+  <si>
+    <t>beta 1</t>
+  </si>
+  <si>
+    <t>lowest losses ever! There is a bit of jaggered lines, so maybe some regularization on top will work</t>
+  </si>
+  <si>
+    <t>increasing beta 1 more</t>
+  </si>
+  <si>
+    <t>lowest losses ever! Let's try even higher beta1 values</t>
+  </si>
+  <si>
+    <t>lowest losses ever! Maybe let's stick with this</t>
+  </si>
+  <si>
+    <t>14 but with regularization</t>
+  </si>
+  <si>
+    <t>a lot of straight lines in plot, what if slightly lower regularization?</t>
+  </si>
+  <si>
+    <t>15 but less regularization</t>
+  </si>
+  <si>
+    <t>l2,0.0001</t>
+  </si>
+  <si>
+    <t>more training of 8</t>
+  </si>
+  <si>
+    <t>larger loss numbers, obviously not the right direction to go, 16 should show more promising results</t>
+  </si>
+  <si>
+    <t>jaggered lines still exist, needs a bit more smoothing, but results is promising as it retained the hook in MS, now to mess with beta 2</t>
+  </si>
+  <si>
+    <t>beta 2</t>
+  </si>
+  <si>
+    <t>16 but less beta 2</t>
   </si>
 </sst>
 </file>
@@ -529,29 +580,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7973A843-EDF6-4158-B183-D0716657A8E3}">
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="12" width="9.7109375" customWidth="1"/>
+    <col min="3" max="14" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>0</v>
@@ -572,22 +623,28 @@
         <v>5</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -610,13 +667,19 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>9211</v>
-      </c>
-      <c r="L4" t="s">
+        <v>0.9</v>
+      </c>
+      <c r="I4">
+        <v>0.999</v>
+      </c>
+      <c r="J4">
+        <v>9211</v>
+      </c>
+      <c r="N4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -639,18 +702,24 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>9211</v>
-      </c>
-      <c r="L5" t="s">
+        <v>0.9</v>
+      </c>
+      <c r="I5">
+        <v>0.999</v>
+      </c>
+      <c r="J5">
+        <v>9211</v>
+      </c>
+      <c r="N5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>0</v>
@@ -670,23 +739,25 @@
       <c r="G8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="N8" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -709,25 +780,31 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <v>9211</v>
+        <v>0.9</v>
       </c>
       <c r="I9">
+        <v>0.999</v>
+      </c>
+      <c r="J9">
+        <v>9211</v>
+      </c>
+      <c r="K9">
         <v>10000</v>
       </c>
-      <c r="J9">
+      <c r="L9">
         <v>3.9449999999999999E-2</v>
       </c>
-      <c r="K9">
+      <c r="M9">
         <v>3.39E-2</v>
       </c>
-      <c r="L9" t="s">
+      <c r="N9" t="s">
         <v>17</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="Q9" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
@@ -750,25 +827,31 @@
         <v>0</v>
       </c>
       <c r="H10">
-        <v>9211</v>
+        <v>0.9</v>
       </c>
       <c r="I10">
+        <v>0.999</v>
+      </c>
+      <c r="J10">
+        <v>9211</v>
+      </c>
+      <c r="K10">
         <v>10000</v>
       </c>
-      <c r="J10">
+      <c r="L10">
         <v>3.7409999999999999E-2</v>
       </c>
-      <c r="K10">
+      <c r="M10">
         <v>4.0899999999999999E-2</v>
       </c>
-      <c r="L10" t="s">
+      <c r="N10" t="s">
         <v>19</v>
       </c>
-      <c r="O10" t="s">
+      <c r="Q10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
@@ -791,25 +874,31 @@
         <v>0</v>
       </c>
       <c r="H11">
-        <v>9211</v>
+        <v>0.9</v>
       </c>
       <c r="I11">
+        <v>0.999</v>
+      </c>
+      <c r="J11">
+        <v>9211</v>
+      </c>
+      <c r="K11">
         <v>10000</v>
       </c>
-      <c r="J11">
+      <c r="L11">
         <v>6.3380000000000006E-2</v>
       </c>
-      <c r="K11">
+      <c r="M11">
         <v>0.1028</v>
       </c>
-      <c r="L11" t="s">
+      <c r="N11" t="s">
         <v>21</v>
       </c>
-      <c r="O11" t="s">
+      <c r="Q11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4</v>
       </c>
@@ -832,22 +921,28 @@
         <v>0</v>
       </c>
       <c r="H12">
-        <v>9211</v>
+        <v>0.9</v>
       </c>
       <c r="I12">
+        <v>0.999</v>
+      </c>
+      <c r="J12">
+        <v>9211</v>
+      </c>
+      <c r="K12">
         <v>20000</v>
       </c>
-      <c r="J12">
+      <c r="L12">
         <v>4.0480000000000002E-2</v>
       </c>
-      <c r="K12">
+      <c r="M12">
         <v>4.9099999999999998E-2</v>
       </c>
-      <c r="L12" t="s">
+      <c r="N12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>5</v>
       </c>
@@ -870,27 +965,33 @@
         <v>0</v>
       </c>
       <c r="H13">
-        <v>9211</v>
+        <v>0.9</v>
       </c>
       <c r="I13">
+        <v>0.999</v>
+      </c>
+      <c r="J13">
+        <v>9211</v>
+      </c>
+      <c r="K13">
         <v>50000</v>
       </c>
-      <c r="J13">
+      <c r="L13">
         <v>0.3609</v>
       </c>
-      <c r="K13">
+      <c r="M13">
         <v>3.9100000000000003E-2</v>
       </c>
-      <c r="L13" t="s">
+      <c r="N13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
         <v>0</v>
@@ -910,23 +1011,25 @@
       <c r="G17" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="K17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="L17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="M17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="N17" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>6</v>
       </c>
@@ -949,22 +1052,28 @@
         <v>0</v>
       </c>
       <c r="H18">
-        <v>9211</v>
+        <v>0.9</v>
       </c>
       <c r="I18">
+        <v>0.999</v>
+      </c>
+      <c r="J18">
+        <v>9211</v>
+      </c>
+      <c r="K18">
         <v>10000</v>
       </c>
-      <c r="J18">
+      <c r="L18">
         <v>2.3470000000000001E-2</v>
       </c>
-      <c r="K18">
+      <c r="M18">
         <v>4.8399999999999999E-2</v>
       </c>
-      <c r="L18" t="s">
+      <c r="N18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>7</v>
       </c>
@@ -987,22 +1096,28 @@
         <v>0</v>
       </c>
       <c r="H19">
-        <v>9211</v>
+        <v>0.9</v>
       </c>
       <c r="I19">
+        <v>0.999</v>
+      </c>
+      <c r="J19">
+        <v>9211</v>
+      </c>
+      <c r="K19">
         <v>50000</v>
       </c>
-      <c r="J19">
+      <c r="L19">
         <v>1.3849999999999999E-2</v>
       </c>
-      <c r="K19">
+      <c r="M19">
         <v>1.89E-2</v>
       </c>
-      <c r="L19" t="s">
+      <c r="N19" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>8</v>
       </c>
@@ -1025,22 +1140,28 @@
         <v>0</v>
       </c>
       <c r="H20">
-        <v>9211</v>
+        <v>0.9</v>
       </c>
       <c r="I20">
+        <v>0.999</v>
+      </c>
+      <c r="J20">
+        <v>9211</v>
+      </c>
+      <c r="K20">
         <v>50000</v>
       </c>
-      <c r="J20">
+      <c r="L20">
         <v>1.0279999999999999E-2</v>
       </c>
-      <c r="K20">
+      <c r="M20">
         <v>1.23E-2</v>
       </c>
-      <c r="L20" t="s">
+      <c r="N20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>9</v>
       </c>
@@ -1063,22 +1184,28 @@
         <v>0</v>
       </c>
       <c r="H21">
-        <v>9211</v>
+        <v>0.9</v>
       </c>
       <c r="I21">
+        <v>0.999</v>
+      </c>
+      <c r="J21">
+        <v>9211</v>
+      </c>
+      <c r="K21">
         <v>50000</v>
       </c>
-      <c r="J21">
+      <c r="L21">
         <v>0.11132</v>
       </c>
-      <c r="K21">
+      <c r="M21">
         <v>9.6299999999999997E-2</v>
       </c>
-      <c r="L21" t="s">
+      <c r="N21" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>10</v>
       </c>
@@ -1101,81 +1228,253 @@
         <v>0</v>
       </c>
       <c r="H22">
-        <v>9211</v>
+        <v>0.9</v>
       </c>
       <c r="I22">
+        <v>0.999</v>
+      </c>
+      <c r="J22">
+        <v>9211</v>
+      </c>
+      <c r="K22">
         <v>250000</v>
       </c>
-      <c r="J22">
+      <c r="L22">
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="K22">
+      <c r="M22">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="L22" t="s">
+      <c r="N22" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>11</v>
+      </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="D23">
+        <v>32</v>
+      </c>
+      <c r="E23">
+        <v>1E-4</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0.99</v>
+      </c>
+      <c r="I23">
+        <v>0.999</v>
+      </c>
+      <c r="J23">
+        <v>9211</v>
+      </c>
+      <c r="K23">
+        <v>10000</v>
+      </c>
+      <c r="L23">
+        <v>2.4799999999999999E-2</v>
+      </c>
+      <c r="M23">
+        <v>2.0199999999999999E-2</v>
+      </c>
+      <c r="N23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>12</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <v>32</v>
+      </c>
+      <c r="E24">
+        <v>1E-4</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0.99</v>
+      </c>
+      <c r="I24">
+        <v>0.999</v>
+      </c>
+      <c r="J24">
+        <v>9211</v>
+      </c>
+      <c r="K24">
+        <v>50000</v>
+      </c>
+      <c r="L24">
+        <v>9.4699999999999993E-3</v>
+      </c>
+      <c r="M24">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="N24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>13</v>
+      </c>
+      <c r="B25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>32</v>
+      </c>
+      <c r="E25">
+        <v>1E-4</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0.999</v>
+      </c>
+      <c r="I25">
+        <v>0.999</v>
+      </c>
+      <c r="J25">
+        <v>9211</v>
+      </c>
+      <c r="K25">
+        <v>50000</v>
+      </c>
+      <c r="L25">
+        <v>5.8999999999999999E-3</v>
+      </c>
+      <c r="M25">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="N25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>14</v>
+      </c>
+      <c r="B26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26">
+        <v>32</v>
+      </c>
+      <c r="E26">
+        <v>1E-4</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="I26">
+        <v>0.999</v>
+      </c>
+      <c r="J26">
+        <v>9211</v>
+      </c>
+      <c r="K26">
+        <v>50000</v>
+      </c>
+      <c r="L26">
+        <v>4.7000000000000002E-3</v>
+      </c>
+      <c r="M26">
+        <v>4.8999999999999998E-3</v>
+      </c>
+      <c r="N26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B27" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="C27">
+        <v>4</v>
+      </c>
+      <c r="D27">
+        <v>32</v>
+      </c>
+      <c r="E27">
+        <v>1E-4</v>
+      </c>
+      <c r="F27" t="s">
+        <v>30</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="I27">
+        <v>0.999</v>
+      </c>
+      <c r="J27">
+        <v>9211</v>
+      </c>
+      <c r="K27">
+        <v>50000</v>
+      </c>
+      <c r="L27">
+        <v>1.469E-2</v>
+      </c>
+      <c r="M27">
+        <v>1.24E-2</v>
+      </c>
+      <c r="N27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="C28">
         <v>4</v>
@@ -1186,34 +1485,40 @@
       <c r="E28">
         <v>1E-4</v>
       </c>
-      <c r="F28">
-        <v>0</v>
+      <c r="F28" t="s">
+        <v>56</v>
       </c>
       <c r="G28">
         <v>0</v>
       </c>
       <c r="H28">
-        <v>4310530</v>
+        <v>0.99990000000000001</v>
       </c>
       <c r="I28">
-        <v>2000</v>
+        <v>0.999</v>
       </c>
       <c r="J28">
-        <v>5.0880000000000002E-2</v>
+        <v>9211</v>
       </c>
       <c r="K28">
-        <v>5.5100000000000003E-2</v>
-      </c>
-      <c r="L28" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+        <v>50000</v>
+      </c>
+      <c r="L28">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="M28">
+        <v>6.6E-3</v>
+      </c>
+      <c r="N28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="C29">
         <v>4</v>
@@ -1224,25 +1529,204 @@
       <c r="E29">
         <v>1E-4</v>
       </c>
-      <c r="F29">
-        <v>0</v>
+      <c r="F29" t="s">
+        <v>30</v>
       </c>
       <c r="G29">
         <v>0</v>
       </c>
       <c r="H29">
+        <v>0.9</v>
+      </c>
+      <c r="I29">
+        <v>0.999</v>
+      </c>
+      <c r="J29">
+        <v>9211</v>
+      </c>
+      <c r="K29">
+        <v>250000</v>
+      </c>
+      <c r="L29">
+        <v>1.9130000000000001E-2</v>
+      </c>
+      <c r="M29">
+        <v>1.6799999999999999E-2</v>
+      </c>
+      <c r="N29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>18</v>
+      </c>
+      <c r="B30" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30">
+        <v>4</v>
+      </c>
+      <c r="D30">
+        <v>32</v>
+      </c>
+      <c r="E30">
+        <v>1E-4</v>
+      </c>
+      <c r="F30" t="s">
+        <v>56</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="I30">
+        <v>0.99</v>
+      </c>
+      <c r="J30">
+        <v>9211</v>
+      </c>
+      <c r="K30">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>2</v>
+      </c>
+      <c r="B36" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36">
+        <v>32</v>
+      </c>
+      <c r="E36">
+        <v>1E-4</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0.9</v>
+      </c>
+      <c r="J36">
         <v>4310530</v>
       </c>
-      <c r="I29">
+      <c r="K36">
+        <v>2000</v>
+      </c>
+      <c r="L36">
+        <v>5.0880000000000002E-2</v>
+      </c>
+      <c r="M36">
+        <v>5.5100000000000003E-2</v>
+      </c>
+      <c r="N36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>3</v>
+      </c>
+      <c r="B37" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37">
+        <v>4</v>
+      </c>
+      <c r="D37">
+        <v>32</v>
+      </c>
+      <c r="E37">
+        <v>1E-4</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>0.9</v>
+      </c>
+      <c r="J37">
+        <v>4310530</v>
+      </c>
+      <c r="K37">
         <v>12000</v>
       </c>
-      <c r="J29">
+      <c r="L37">
         <v>4.6289999999999998E-2</v>
       </c>
-      <c r="K29">
+      <c r="M37">
         <v>5.21E-2</v>
       </c>
-      <c r="L29" t="s">
+      <c r="N37" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Grid NN: notes spreadsheet with updates for numbers on trials 18-27
</commit_message>
<xml_diff>
--- a/Hin's_files/NNgrids_notes.xlsx
+++ b/Hin's_files/NNgrids_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\UoB physics stuff\year 4\FYP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0548801-4359-45CA-824F-341F4D28A0AF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15EBAADF-AD0C-4DCD-8A6E-8C0358065B46}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{27E1F3F0-F425-4B4B-8745-3E9458FE7065}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="84">
   <si>
     <t>details</t>
   </si>
@@ -217,6 +217,72 @@
   </si>
   <si>
     <t>16 but less beta 2</t>
+  </si>
+  <si>
+    <t>doing less good compared to 16, lets try more beta 2 instead</t>
+  </si>
+  <si>
+    <t>16 but more beta 2</t>
+  </si>
+  <si>
+    <t>very low loss, but looking at the HR plot, it seems the plot was smoothed out too much, losing some bumps in the MS hook. I would suggest to just use the original beta_2=0.999 value</t>
+  </si>
+  <si>
+    <t>log10(M, Age, feh, MLT) -&gt; log10(L, Teff, delnu) (all ages)</t>
+  </si>
+  <si>
+    <t>flattened MS hooks, overall okish fit, age vs delnu is more jaggered than data, loss still decreasing, more training</t>
+  </si>
+  <si>
+    <t>more training of 20</t>
+  </si>
+  <si>
+    <t>lowest eval loss ever! HR diagram looks very good now, loss still steadily decreasing, more training is needed</t>
+  </si>
+  <si>
+    <t>increasing archetecture</t>
+  </si>
+  <si>
+    <t>L dex</t>
+  </si>
+  <si>
+    <t>Teff dex</t>
+  </si>
+  <si>
+    <t>delnu dex</t>
+  </si>
+  <si>
+    <t>lowest loss ever! Some parts of HR diagram is flattened (hook) but error is still going down, so can train more (or increase architecture more)</t>
+  </si>
+  <si>
+    <t>lowest loss ever! Error is still going down, so can train more. HR diagram is jaggered. This took 8.5 hours to train, twice as much as 22, don’t know if should use bigger or smaller architectures</t>
+  </si>
+  <si>
+    <t>higher lr from 20</t>
+  </si>
+  <si>
+    <t>more layers and higher lr from 22</t>
+  </si>
+  <si>
+    <t>higher lr from 25</t>
+  </si>
+  <si>
+    <t>lower final learning loss than 20, with the same number of epochs, HR looks better than 20, not overfitting yet, try increase lr even further</t>
+  </si>
+  <si>
+    <t>lower final learning loss than 25, with the same number of epochs, HR looks better than 25, not overfitting yet, try increase lr even further</t>
+  </si>
+  <si>
+    <t>higher lr from 26</t>
+  </si>
+  <si>
+    <t>straight line segments in HR plot, high loss, bad result, 0.01 lr is probably the best</t>
+  </si>
+  <si>
+    <t>super big architecture = good, lowest loss, dex wtever across the board, repeat for 500k epochs to search for overfitting</t>
+  </si>
+  <si>
+    <t>more training of 24</t>
   </si>
 </sst>
 </file>
@@ -240,18 +306,33 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -260,12 +341,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,10 +668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7973A843-EDF6-4158-B183-D0716657A8E3}">
-  <dimension ref="A1:Q37"/>
+  <dimension ref="A1:Q71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="L44" sqref="L44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,11 +684,13 @@
       <c r="A1" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
+      <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -631,7 +721,7 @@
       <c r="J3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="L3" s="1" t="s">
@@ -675,6 +765,7 @@
       <c r="J4">
         <v>9211</v>
       </c>
+      <c r="K4" s="3"/>
       <c r="N4" t="s">
         <v>12</v>
       </c>
@@ -710,14 +801,19 @@
       <c r="J5">
         <v>9211</v>
       </c>
+      <c r="K5" s="3"/>
       <c r="N5" t="s">
         <v>12</v>
       </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K6" s="3"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>37</v>
       </c>
+      <c r="K7" s="3"/>
     </row>
     <row r="8" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
@@ -739,12 +835,16 @@
       <c r="G8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+      <c r="H8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="J8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="K8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="L8" s="1" t="s">
@@ -788,7 +888,7 @@
       <c r="J9">
         <v>9211</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="3">
         <v>10000</v>
       </c>
       <c r="L9">
@@ -835,7 +935,7 @@
       <c r="J10">
         <v>9211</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="3">
         <v>10000</v>
       </c>
       <c r="L10">
@@ -882,7 +982,7 @@
       <c r="J11">
         <v>9211</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="3">
         <v>10000</v>
       </c>
       <c r="L11">
@@ -929,7 +1029,7 @@
       <c r="J12">
         <v>9211</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="3">
         <v>20000</v>
       </c>
       <c r="L12">
@@ -973,7 +1073,7 @@
       <c r="J13">
         <v>9211</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="3">
         <v>50000</v>
       </c>
       <c r="L13">
@@ -985,11 +1085,18 @@
       <c r="N13" t="s">
         <v>25</v>
       </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K15" s="3"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>36</v>
       </c>
+      <c r="K16" s="3"/>
     </row>
     <row r="17" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
@@ -1011,12 +1118,16 @@
       <c r="G17" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
+      <c r="H17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="J17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="K17" s="4" t="s">
         <v>7</v>
       </c>
       <c r="L17" s="1" t="s">
@@ -1060,7 +1171,7 @@
       <c r="J18">
         <v>9211</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="3">
         <v>10000</v>
       </c>
       <c r="L18">
@@ -1104,7 +1215,7 @@
       <c r="J19">
         <v>9211</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="3">
         <v>50000</v>
       </c>
       <c r="L19">
@@ -1148,7 +1259,7 @@
       <c r="J20">
         <v>9211</v>
       </c>
-      <c r="K20">
+      <c r="K20" s="3">
         <v>50000</v>
       </c>
       <c r="L20">
@@ -1192,7 +1303,7 @@
       <c r="J21">
         <v>9211</v>
       </c>
-      <c r="K21">
+      <c r="K21" s="3">
         <v>50000</v>
       </c>
       <c r="L21">
@@ -1209,7 +1320,7 @@
       <c r="A22">
         <v>10</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="7" t="s">
         <v>43</v>
       </c>
       <c r="C22">
@@ -1236,7 +1347,7 @@
       <c r="J22">
         <v>9211</v>
       </c>
-      <c r="K22">
+      <c r="K22" s="3">
         <v>250000</v>
       </c>
       <c r="L22">
@@ -1280,7 +1391,7 @@
       <c r="J23">
         <v>9211</v>
       </c>
-      <c r="K23">
+      <c r="K23" s="3">
         <v>10000</v>
       </c>
       <c r="L23">
@@ -1324,7 +1435,7 @@
       <c r="J24">
         <v>9211</v>
       </c>
-      <c r="K24">
+      <c r="K24" s="3">
         <v>50000</v>
       </c>
       <c r="L24">
@@ -1368,7 +1479,7 @@
       <c r="J25">
         <v>9211</v>
       </c>
-      <c r="K25">
+      <c r="K25" s="3">
         <v>50000</v>
       </c>
       <c r="L25">
@@ -1412,7 +1523,7 @@
       <c r="J26">
         <v>9211</v>
       </c>
-      <c r="K26">
+      <c r="K26" s="3">
         <v>50000</v>
       </c>
       <c r="L26">
@@ -1456,7 +1567,7 @@
       <c r="J27">
         <v>9211</v>
       </c>
-      <c r="K27">
+      <c r="K27" s="3">
         <v>50000</v>
       </c>
       <c r="L27">
@@ -1500,7 +1611,7 @@
       <c r="J28">
         <v>9211</v>
       </c>
-      <c r="K28">
+      <c r="K28" s="3">
         <v>50000</v>
       </c>
       <c r="L28">
@@ -1517,7 +1628,7 @@
       <c r="A29">
         <v>17</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C29">
@@ -1544,7 +1655,7 @@
       <c r="J29">
         <v>9211</v>
       </c>
-      <c r="K29">
+      <c r="K29" s="3">
         <v>250000</v>
       </c>
       <c r="L29">
@@ -1588,69 +1699,128 @@
       <c r="J30">
         <v>9211</v>
       </c>
-      <c r="K30">
+      <c r="K30" s="3">
         <v>50000</v>
       </c>
+      <c r="L30">
+        <v>1.2E-2</v>
+      </c>
+      <c r="M30">
+        <v>8.3000000000000001E-3</v>
+      </c>
+      <c r="N30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>19</v>
+      </c>
+      <c r="B31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31">
+        <v>4</v>
+      </c>
+      <c r="D31">
+        <v>32</v>
+      </c>
+      <c r="E31">
+        <v>1E-4</v>
+      </c>
+      <c r="F31" t="s">
+        <v>56</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="I31">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="J31">
+        <v>9211</v>
+      </c>
+      <c r="K31" s="3">
+        <v>50000</v>
+      </c>
+      <c r="L31">
+        <v>8.3400000000000002E-3</v>
+      </c>
+      <c r="M31">
+        <v>4.8999999999999998E-3</v>
+      </c>
+      <c r="N31" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C34" s="1" t="s">
+      <c r="K32" s="3"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K33" s="3"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>65</v>
+      </c>
+      <c r="K34" s="3"/>
+    </row>
+    <row r="35" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F34" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G34" s="1" t="s">
+      <c r="F35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G35" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1" t="s">
+      <c r="H35" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J35" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K34" s="1" t="s">
+      <c r="K35" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L34" s="1" t="s">
+      <c r="L35" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M34" s="1" t="s">
+      <c r="M35" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N34" s="1" t="s">
+      <c r="N35" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="O35" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="P35" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q35" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>1</v>
-      </c>
-      <c r="B35" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B36" t="s">
         <v>11</v>
@@ -1664,37 +1834,40 @@
       <c r="E36">
         <v>1E-4</v>
       </c>
-      <c r="F36">
-        <v>0</v>
+      <c r="F36" t="s">
+        <v>56</v>
       </c>
       <c r="G36">
         <v>0</v>
       </c>
       <c r="H36">
-        <v>0.9</v>
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="I36">
+        <v>0.999</v>
       </c>
       <c r="J36">
-        <v>4310530</v>
-      </c>
-      <c r="K36">
-        <v>2000</v>
+        <v>9211</v>
+      </c>
+      <c r="K36" s="3">
+        <v>50000</v>
       </c>
       <c r="L36">
-        <v>5.0880000000000002E-2</v>
+        <v>9.9900000000000006E-3</v>
       </c>
       <c r="M36">
-        <v>5.5100000000000003E-2</v>
-      </c>
-      <c r="N36" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="C37">
         <v>4</v>
@@ -1705,30 +1878,614 @@
       <c r="E37">
         <v>1E-4</v>
       </c>
-      <c r="F37">
-        <v>0</v>
+      <c r="F37" t="s">
+        <v>56</v>
       </c>
       <c r="G37">
         <v>0</v>
       </c>
       <c r="H37">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="I37">
+        <v>0.999</v>
+      </c>
+      <c r="J37">
+        <v>9211</v>
+      </c>
+      <c r="K37" s="3">
+        <v>100000</v>
+      </c>
+      <c r="L37">
+        <v>5.4400000000000004E-3</v>
+      </c>
+      <c r="M37">
+        <v>3.8E-3</v>
+      </c>
+      <c r="N37">
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="O37">
+        <v>4.8999999999999998E-3</v>
+      </c>
+      <c r="P37">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>22</v>
+      </c>
+      <c r="B38" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38">
+        <v>4</v>
+      </c>
+      <c r="D38">
+        <v>128</v>
+      </c>
+      <c r="E38">
+        <v>1E-4</v>
+      </c>
+      <c r="F38" t="s">
+        <v>56</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="I38">
+        <v>0.999</v>
+      </c>
+      <c r="J38">
+        <v>9211</v>
+      </c>
+      <c r="K38" s="3">
+        <v>50000</v>
+      </c>
+      <c r="L38">
+        <v>4.4400000000000004E-3</v>
+      </c>
+      <c r="M38">
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="N38">
+        <v>1.55E-2</v>
+      </c>
+      <c r="O38">
+        <v>4.3E-3</v>
+      </c>
+      <c r="P38">
+        <v>1.129E-2</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>23</v>
+      </c>
+      <c r="B39" t="s">
+        <v>69</v>
+      </c>
+      <c r="C39">
+        <v>4</v>
+      </c>
+      <c r="D39">
+        <v>256</v>
+      </c>
+      <c r="E39">
+        <v>1E-4</v>
+      </c>
+      <c r="F39" t="s">
+        <v>56</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="I39">
+        <v>0.999</v>
+      </c>
+      <c r="J39">
+        <v>9211</v>
+      </c>
+      <c r="K39" s="3">
+        <v>50000</v>
+      </c>
+      <c r="L39">
+        <v>3.8449999999999999E-3</v>
+      </c>
+      <c r="M39">
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="N39">
+        <v>1.3480000000000001E-2</v>
+      </c>
+      <c r="O39">
+        <v>3.336E-3</v>
+      </c>
+      <c r="P39">
+        <v>1.0149999999999999E-2</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>24</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40">
+        <v>8</v>
+      </c>
+      <c r="D40">
+        <v>128</v>
+      </c>
+      <c r="E40">
+        <v>1E-3</v>
+      </c>
+      <c r="F40" t="s">
+        <v>56</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="I40">
+        <v>0.999</v>
+      </c>
+      <c r="J40">
+        <v>9211</v>
+      </c>
+      <c r="K40" s="3">
+        <v>50000</v>
+      </c>
+      <c r="L40" s="5">
+        <v>1.0430000000000001E-3</v>
+      </c>
+      <c r="M40" s="6">
+        <v>9.3528999999999997E-4</v>
+      </c>
+      <c r="N40">
+        <v>3.7716009999999999E-3</v>
+      </c>
+      <c r="O40">
+        <v>1.087382E-3</v>
+      </c>
+      <c r="P40">
+        <v>2.3932962000000001E-3</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>25</v>
+      </c>
+      <c r="B41" t="s">
+        <v>75</v>
+      </c>
+      <c r="C41">
+        <v>4</v>
+      </c>
+      <c r="D41">
+        <v>32</v>
+      </c>
+      <c r="E41">
+        <v>1E-3</v>
+      </c>
+      <c r="F41" t="s">
+        <v>56</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="I41">
+        <v>0.999</v>
+      </c>
+      <c r="J41">
+        <v>9211</v>
+      </c>
+      <c r="K41" s="3">
+        <v>50000</v>
+      </c>
+      <c r="L41">
+        <v>7.5900000000000004E-3</v>
+      </c>
+      <c r="M41">
+        <v>6.7000000000000002E-3</v>
+      </c>
+      <c r="N41">
+        <v>2.6599999999999999E-2</v>
+      </c>
+      <c r="O41">
+        <v>8.1499999999999993E-3</v>
+      </c>
+      <c r="P41">
+        <v>1.83E-2</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>26</v>
+      </c>
+      <c r="B42" t="s">
+        <v>77</v>
+      </c>
+      <c r="C42">
+        <v>4</v>
+      </c>
+      <c r="D42">
+        <v>32</v>
+      </c>
+      <c r="E42">
+        <v>0.01</v>
+      </c>
+      <c r="F42" t="s">
+        <v>56</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="I42">
+        <v>0.999</v>
+      </c>
+      <c r="J42">
+        <v>9211</v>
+      </c>
+      <c r="K42" s="3">
+        <v>50000</v>
+      </c>
+      <c r="L42" s="5">
+        <v>5.0200000000000002E-3</v>
+      </c>
+      <c r="M42" s="5">
+        <v>3.8E-3</v>
+      </c>
+      <c r="N42" s="5">
+        <v>1.7690000000000001E-2</v>
+      </c>
+      <c r="O42" s="5">
+        <v>4.4169999999999999E-3</v>
+      </c>
+      <c r="P42" s="5">
+        <v>1.278E-2</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>27</v>
+      </c>
+      <c r="B43" t="s">
+        <v>80</v>
+      </c>
+      <c r="C43">
+        <v>4</v>
+      </c>
+      <c r="D43">
+        <v>32</v>
+      </c>
+      <c r="E43">
+        <v>0.1</v>
+      </c>
+      <c r="F43" t="s">
+        <v>56</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="I43">
+        <v>0.999</v>
+      </c>
+      <c r="J43">
+        <v>9211</v>
+      </c>
+      <c r="K43" s="3">
+        <v>50000</v>
+      </c>
+      <c r="L43" s="5">
+        <v>2.47E-2</v>
+      </c>
+      <c r="M43" s="5">
+        <v>1.8700000000000001E-2</v>
+      </c>
+      <c r="N43" s="5">
+        <v>7.4200000000000002E-2</v>
+      </c>
+      <c r="O43" s="5">
+        <v>3.3700000000000001E-2</v>
+      </c>
+      <c r="P43" s="5">
+        <v>6.5799999999999997E-2</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>28</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C44">
+        <v>8</v>
+      </c>
+      <c r="D44">
+        <v>128</v>
+      </c>
+      <c r="E44">
+        <v>1E-3</v>
+      </c>
+      <c r="F44" t="s">
+        <v>56</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="I44">
+        <v>0.999</v>
+      </c>
+      <c r="J44">
+        <v>9211</v>
+      </c>
+      <c r="K44" s="3">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K45" s="3"/>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K46" s="3"/>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>36</v>
+      </c>
+      <c r="K47" s="3"/>
+    </row>
+    <row r="48" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K48" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M48" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N48" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49" t="s">
+        <v>41</v>
+      </c>
+      <c r="K49" s="3"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>2</v>
+      </c>
+      <c r="B50" t="s">
+        <v>11</v>
+      </c>
+      <c r="C50">
+        <v>4</v>
+      </c>
+      <c r="D50">
+        <v>32</v>
+      </c>
+      <c r="E50">
+        <v>1E-4</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
         <v>0.9</v>
       </c>
-      <c r="J37">
+      <c r="I50">
+        <v>0.999</v>
+      </c>
+      <c r="J50">
         <v>4310530</v>
       </c>
-      <c r="K37">
+      <c r="K50" s="3">
+        <v>2000</v>
+      </c>
+      <c r="L50">
+        <v>5.0880000000000002E-2</v>
+      </c>
+      <c r="M50">
+        <v>5.5100000000000003E-2</v>
+      </c>
+      <c r="N50" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>3</v>
+      </c>
+      <c r="B51" t="s">
+        <v>40</v>
+      </c>
+      <c r="C51">
+        <v>4</v>
+      </c>
+      <c r="D51">
+        <v>32</v>
+      </c>
+      <c r="E51">
+        <v>1E-4</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>0.9</v>
+      </c>
+      <c r="I51">
+        <v>0.999</v>
+      </c>
+      <c r="J51">
+        <v>4310530</v>
+      </c>
+      <c r="K51" s="3">
         <v>12000</v>
       </c>
-      <c r="L37">
+      <c r="L51">
         <v>4.6289999999999998E-2</v>
       </c>
-      <c r="M37">
+      <c r="M51">
         <v>5.21E-2</v>
       </c>
-      <c r="N37" t="s">
+      <c r="N51" t="s">
         <v>42</v>
       </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="K52" s="3"/>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K53" s="3"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K54" s="3"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K55" s="3"/>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K56" s="3"/>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K57" s="3"/>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K58" s="3"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K59" s="3"/>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K60" s="3"/>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K61" s="3"/>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K62" s="3"/>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K63" s="3"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K64" s="3"/>
+    </row>
+    <row r="65" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K65" s="3"/>
+    </row>
+    <row r="66" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K66" s="3"/>
+    </row>
+    <row r="67" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K67" s="3"/>
+    </row>
+    <row r="68" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K68" s="3"/>
+    </row>
+    <row r="69" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K69" s="3"/>
+    </row>
+    <row r="70" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K70" s="3"/>
+    </row>
+    <row r="71" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K71" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added big grid runs 4-11 hyperparameter and results
Comment: all runs are still bad and have not achieved satisfactory accuracy
</commit_message>
<xml_diff>
--- a/Hin's_files/NNgrids_notes.xlsx
+++ b/Hin's_files/NNgrids_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\UoB physics stuff\year 4\FYP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15EBAADF-AD0C-4DCD-8A6E-8C0358065B46}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E449D7-0FF5-40E9-BCC9-3C14064B7D57}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{27E1F3F0-F425-4B4B-8745-3E9458FE7065}"/>
+    <workbookView xWindow="14550" yWindow="2490" windowWidth="5940" windowHeight="7965" xr2:uid="{27E1F3F0-F425-4B4B-8745-3E9458FE7065}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="112">
   <si>
     <t>details</t>
   </si>
@@ -283,6 +283,90 @@
   </si>
   <si>
     <t>more training of 24</t>
+  </si>
+  <si>
+    <t>best results so far! Training flatterns off, dex is well within target, this is as good as we can do with the small grid. Work with small grid is done.</t>
+  </si>
+  <si>
+    <t>activation function</t>
+  </si>
+  <si>
+    <t>relu</t>
+  </si>
+  <si>
+    <t>elu</t>
+  </si>
+  <si>
+    <t>using elu for HBM</t>
+  </si>
+  <si>
+    <t>bad</t>
+  </si>
+  <si>
+    <t>more training of 29</t>
+  </si>
+  <si>
+    <t>increasing archetecture of 29</t>
+  </si>
+  <si>
+    <t>still bad</t>
+  </si>
+  <si>
+    <t>amazing</t>
+  </si>
+  <si>
+    <t>Big stellar evo grid</t>
+  </si>
+  <si>
+    <t>log10(M, Age, 10**feh, Y, MLT) -&gt; log10(L, Teff, delnu)</t>
+  </si>
+  <si>
+    <t>enlarging archetecture</t>
+  </si>
+  <si>
+    <t>bad, and very little improvement</t>
+  </si>
+  <si>
+    <t>resetting lr of 6</t>
+  </si>
+  <si>
+    <t>1.2mil</t>
+  </si>
+  <si>
+    <t>lowering lr and 0ing regularization</t>
+  </si>
+  <si>
+    <t>l2,0.0002</t>
+  </si>
+  <si>
+    <t>l2,0.0003</t>
+  </si>
+  <si>
+    <t>l2,0.0004</t>
+  </si>
+  <si>
+    <t>very very wrong</t>
+  </si>
+  <si>
+    <t>log10(M, Age, 10**feh, Y, MLT) -&gt; log10(radius, Teff/5000, delnu)</t>
+  </si>
+  <si>
+    <t>radius dex</t>
+  </si>
+  <si>
+    <t>bad but slight improvement, though loss has flatterned, will try to 50k epoch</t>
+  </si>
+  <si>
+    <t>more training of 9</t>
+  </si>
+  <si>
+    <t>much better, rather weak at RGB, training loss seems to only go down after 20k, epochs, try bigger archetacture but also to 50k epochs</t>
+  </si>
+  <si>
+    <t>bigger archetecture but more training</t>
+  </si>
+  <si>
+    <t>slightly better, quite wobbly overall, maybe should introduce dropout, loss was still slowly decreasing</t>
   </si>
 </sst>
 </file>
@@ -341,7 +425,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -354,6 +438,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -668,31 +753,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7973A843-EDF6-4158-B183-D0716657A8E3}">
-  <dimension ref="A1:Q71"/>
+  <dimension ref="A1:R72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="L44" sqref="L44"/>
+    <sheetView tabSelected="1" topLeftCell="J61" workbookViewId="0">
+      <selection activeCell="F73" sqref="F73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="14" width="9.7109375" customWidth="1"/>
+    <col min="3" max="15" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="3"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L1" s="3"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
-      <c r="K2" s="3"/>
-    </row>
-    <row r="3" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>0</v>
@@ -704,37 +789,40 @@
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="G3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="L3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -747,30 +835,33 @@
       <c r="D4">
         <v>32</v>
       </c>
-      <c r="E4">
+      <c r="E4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F4">
         <v>1E-3</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
         <v>0.9</v>
       </c>
-      <c r="I4">
-        <v>0.999</v>
-      </c>
       <c r="J4">
+        <v>0.999</v>
+      </c>
+      <c r="K4">
         <v>9211</v>
       </c>
-      <c r="K4" s="3"/>
-      <c r="N4" t="s">
+      <c r="L4" s="3"/>
+      <c r="O4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -783,39 +874,42 @@
       <c r="D5">
         <v>128</v>
       </c>
-      <c r="E5">
+      <c r="E5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F5">
         <v>1E-3</v>
       </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
         <v>0.9</v>
       </c>
-      <c r="I5">
-        <v>0.999</v>
-      </c>
       <c r="J5">
+        <v>0.999</v>
+      </c>
+      <c r="K5">
         <v>9211</v>
       </c>
-      <c r="K5" s="3"/>
-      <c r="N5" t="s">
+      <c r="L5" s="3"/>
+      <c r="O5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="K6" s="3"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>37</v>
       </c>
-      <c r="K7" s="3"/>
-    </row>
-    <row r="8" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>0</v>
@@ -827,37 +921,40 @@
         <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="G8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="L8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="N8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="O8" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -870,41 +967,44 @@
       <c r="D9">
         <v>32</v>
       </c>
-      <c r="E9">
+      <c r="E9" t="s">
+        <v>86</v>
+      </c>
+      <c r="F9">
         <v>1E-3</v>
       </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
         <v>0.9</v>
       </c>
-      <c r="I9">
-        <v>0.999</v>
-      </c>
       <c r="J9">
+        <v>0.999</v>
+      </c>
+      <c r="K9">
         <v>9211</v>
       </c>
-      <c r="K9" s="3">
+      <c r="L9" s="3">
         <v>10000</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>3.9449999999999999E-2</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>3.39E-2</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>17</v>
       </c>
-      <c r="Q9" s="1" t="s">
+      <c r="R9" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
@@ -917,41 +1017,44 @@
       <c r="D10">
         <v>32</v>
       </c>
-      <c r="E10">
+      <c r="E10" t="s">
+        <v>86</v>
+      </c>
+      <c r="F10">
         <v>1E-4</v>
       </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
         <v>0.9</v>
       </c>
-      <c r="I10">
-        <v>0.999</v>
-      </c>
       <c r="J10">
+        <v>0.999</v>
+      </c>
+      <c r="K10">
         <v>9211</v>
       </c>
-      <c r="K10" s="3">
+      <c r="L10" s="3">
         <v>10000</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>3.7409999999999999E-2</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>4.0899999999999999E-2</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>19</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="R10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
@@ -964,41 +1067,44 @@
       <c r="D11">
         <v>32</v>
       </c>
-      <c r="E11">
+      <c r="E11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F11">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
         <v>0.9</v>
       </c>
-      <c r="I11">
-        <v>0.999</v>
-      </c>
       <c r="J11">
+        <v>0.999</v>
+      </c>
+      <c r="K11">
         <v>9211</v>
       </c>
-      <c r="K11" s="3">
+      <c r="L11" s="3">
         <v>10000</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>6.3380000000000006E-2</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>0.1028</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>21</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="R11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4</v>
       </c>
@@ -1011,38 +1117,41 @@
       <c r="D12">
         <v>32</v>
       </c>
-      <c r="E12">
+      <c r="E12" t="s">
+        <v>86</v>
+      </c>
+      <c r="F12">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
         <v>0.9</v>
       </c>
-      <c r="I12">
-        <v>0.999</v>
-      </c>
       <c r="J12">
+        <v>0.999</v>
+      </c>
+      <c r="K12">
         <v>9211</v>
       </c>
-      <c r="K12" s="3">
+      <c r="L12" s="3">
         <v>20000</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>4.0480000000000002E-2</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>4.9099999999999998E-2</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>5</v>
       </c>
@@ -1055,50 +1164,53 @@
       <c r="D13">
         <v>32</v>
       </c>
-      <c r="E13">
+      <c r="E13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F13">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
         <v>0.9</v>
       </c>
-      <c r="I13">
-        <v>0.999</v>
-      </c>
       <c r="J13">
+        <v>0.999</v>
+      </c>
+      <c r="K13">
         <v>9211</v>
       </c>
-      <c r="K13" s="3">
+      <c r="L13" s="3">
         <v>50000</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>0.3609</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>3.9100000000000003E-2</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="K14" s="3"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="K15" s="3"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>36</v>
       </c>
-      <c r="K16" s="3"/>
-    </row>
-    <row r="17" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="L16" s="3"/>
+    </row>
+    <row r="17" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
         <v>0</v>
@@ -1110,37 +1222,40 @@
         <v>2</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="G17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="I17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="K17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K17" s="4" t="s">
+      <c r="L17" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="M17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M17" s="1" t="s">
+      <c r="N17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N17" s="1" t="s">
+      <c r="O17" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>6</v>
       </c>
@@ -1153,38 +1268,41 @@
       <c r="D18">
         <v>32</v>
       </c>
-      <c r="E18">
+      <c r="E18" t="s">
+        <v>86</v>
+      </c>
+      <c r="F18">
         <v>1E-4</v>
       </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
         <v>0.9</v>
       </c>
-      <c r="I18">
-        <v>0.999</v>
-      </c>
       <c r="J18">
+        <v>0.999</v>
+      </c>
+      <c r="K18">
         <v>9211</v>
       </c>
-      <c r="K18" s="3">
+      <c r="L18" s="3">
         <v>10000</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <v>2.3470000000000001E-2</v>
       </c>
-      <c r="M18">
+      <c r="N18">
         <v>4.8399999999999999E-2</v>
       </c>
-      <c r="N18" t="s">
+      <c r="O18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>7</v>
       </c>
@@ -1197,38 +1315,41 @@
       <c r="D19">
         <v>32</v>
       </c>
-      <c r="E19">
+      <c r="E19" t="s">
+        <v>86</v>
+      </c>
+      <c r="F19">
         <v>1E-4</v>
       </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
       <c r="G19">
         <v>0</v>
       </c>
       <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
         <v>0.9</v>
       </c>
-      <c r="I19">
-        <v>0.999</v>
-      </c>
       <c r="J19">
+        <v>0.999</v>
+      </c>
+      <c r="K19">
         <v>9211</v>
       </c>
-      <c r="K19" s="3">
+      <c r="L19" s="3">
         <v>50000</v>
       </c>
-      <c r="L19">
+      <c r="M19">
         <v>1.3849999999999999E-2</v>
       </c>
-      <c r="M19">
+      <c r="N19">
         <v>1.89E-2</v>
       </c>
-      <c r="N19" t="s">
+      <c r="O19" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>8</v>
       </c>
@@ -1241,38 +1362,41 @@
       <c r="D20">
         <v>32</v>
       </c>
-      <c r="E20">
+      <c r="E20" t="s">
+        <v>86</v>
+      </c>
+      <c r="F20">
         <v>1E-4</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>30</v>
       </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
       <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
         <v>0.9</v>
       </c>
-      <c r="I20">
-        <v>0.999</v>
-      </c>
       <c r="J20">
+        <v>0.999</v>
+      </c>
+      <c r="K20">
         <v>9211</v>
       </c>
-      <c r="K20" s="3">
+      <c r="L20" s="3">
         <v>50000</v>
       </c>
-      <c r="L20">
+      <c r="M20">
         <v>1.0279999999999999E-2</v>
       </c>
-      <c r="M20">
+      <c r="N20">
         <v>1.23E-2</v>
       </c>
-      <c r="N20" t="s">
+      <c r="O20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>9</v>
       </c>
@@ -1285,38 +1409,41 @@
       <c r="D21">
         <v>32</v>
       </c>
-      <c r="E21">
+      <c r="E21" t="s">
+        <v>86</v>
+      </c>
+      <c r="F21">
         <v>1E-4</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>32</v>
       </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
       <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
         <v>0.9</v>
       </c>
-      <c r="I21">
-        <v>0.999</v>
-      </c>
       <c r="J21">
+        <v>0.999</v>
+      </c>
+      <c r="K21">
         <v>9211</v>
       </c>
-      <c r="K21" s="3">
+      <c r="L21" s="3">
         <v>50000</v>
       </c>
-      <c r="L21">
+      <c r="M21">
         <v>0.11132</v>
       </c>
-      <c r="M21">
+      <c r="N21">
         <v>9.6299999999999997E-2</v>
       </c>
-      <c r="N21" t="s">
+      <c r="O21" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>10</v>
       </c>
@@ -1329,38 +1456,41 @@
       <c r="D22">
         <v>32</v>
       </c>
-      <c r="E22">
+      <c r="E22" t="s">
+        <v>86</v>
+      </c>
+      <c r="F22">
         <v>1E-4</v>
       </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
       <c r="G22">
         <v>0</v>
       </c>
       <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
         <v>0.9</v>
       </c>
-      <c r="I22">
-        <v>0.999</v>
-      </c>
       <c r="J22">
+        <v>0.999</v>
+      </c>
+      <c r="K22">
         <v>9211</v>
       </c>
-      <c r="K22" s="3">
+      <c r="L22" s="3">
         <v>250000</v>
       </c>
-      <c r="L22">
+      <c r="M22">
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="M22">
+      <c r="N22">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="N22" t="s">
+      <c r="O22" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>11</v>
       </c>
@@ -1373,38 +1503,41 @@
       <c r="D23">
         <v>32</v>
       </c>
-      <c r="E23">
+      <c r="E23" t="s">
+        <v>86</v>
+      </c>
+      <c r="F23">
         <v>1E-4</v>
       </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
       <c r="G23">
         <v>0</v>
       </c>
       <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
         <v>0.99</v>
       </c>
-      <c r="I23">
-        <v>0.999</v>
-      </c>
       <c r="J23">
+        <v>0.999</v>
+      </c>
+      <c r="K23">
         <v>9211</v>
       </c>
-      <c r="K23" s="3">
+      <c r="L23" s="3">
         <v>10000</v>
       </c>
-      <c r="L23">
+      <c r="M23">
         <v>2.4799999999999999E-2</v>
       </c>
-      <c r="M23">
+      <c r="N23">
         <v>2.0199999999999999E-2</v>
       </c>
-      <c r="N23" t="s">
+      <c r="O23" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>12</v>
       </c>
@@ -1417,38 +1550,41 @@
       <c r="D24">
         <v>32</v>
       </c>
-      <c r="E24">
+      <c r="E24" t="s">
+        <v>86</v>
+      </c>
+      <c r="F24">
         <v>1E-4</v>
       </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
       <c r="G24">
         <v>0</v>
       </c>
       <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
         <v>0.99</v>
       </c>
-      <c r="I24">
-        <v>0.999</v>
-      </c>
       <c r="J24">
+        <v>0.999</v>
+      </c>
+      <c r="K24">
         <v>9211</v>
       </c>
-      <c r="K24" s="3">
+      <c r="L24" s="3">
         <v>50000</v>
       </c>
-      <c r="L24">
+      <c r="M24">
         <v>9.4699999999999993E-3</v>
       </c>
-      <c r="M24">
+      <c r="N24">
         <v>7.7000000000000002E-3</v>
       </c>
-      <c r="N24" t="s">
+      <c r="O24" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>13</v>
       </c>
@@ -1461,38 +1597,41 @@
       <c r="D25">
         <v>32</v>
       </c>
-      <c r="E25">
+      <c r="E25" t="s">
+        <v>86</v>
+      </c>
+      <c r="F25">
         <v>1E-4</v>
       </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
       <c r="G25">
         <v>0</v>
       </c>
       <c r="H25">
-        <v>0.999</v>
+        <v>0</v>
       </c>
       <c r="I25">
         <v>0.999</v>
       </c>
       <c r="J25">
+        <v>0.999</v>
+      </c>
+      <c r="K25">
         <v>9211</v>
       </c>
-      <c r="K25" s="3">
+      <c r="L25" s="3">
         <v>50000</v>
       </c>
-      <c r="L25">
+      <c r="M25">
         <v>5.8999999999999999E-3</v>
       </c>
-      <c r="M25">
+      <c r="N25">
         <v>5.1999999999999998E-3</v>
       </c>
-      <c r="N25" t="s">
+      <c r="O25" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>14</v>
       </c>
@@ -1505,38 +1644,41 @@
       <c r="D26">
         <v>32</v>
       </c>
-      <c r="E26">
+      <c r="E26" t="s">
+        <v>86</v>
+      </c>
+      <c r="F26">
         <v>1E-4</v>
       </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
       <c r="G26">
         <v>0</v>
       </c>
       <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
         <v>0.99990000000000001</v>
       </c>
-      <c r="I26">
-        <v>0.999</v>
-      </c>
       <c r="J26">
+        <v>0.999</v>
+      </c>
+      <c r="K26">
         <v>9211</v>
       </c>
-      <c r="K26" s="3">
+      <c r="L26" s="3">
         <v>50000</v>
       </c>
-      <c r="L26">
+      <c r="M26">
         <v>4.7000000000000002E-3</v>
       </c>
-      <c r="M26">
+      <c r="N26">
         <v>4.8999999999999998E-3</v>
       </c>
-      <c r="N26" t="s">
+      <c r="O26" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>15</v>
       </c>
@@ -1549,38 +1691,41 @@
       <c r="D27">
         <v>32</v>
       </c>
-      <c r="E27">
+      <c r="E27" t="s">
+        <v>86</v>
+      </c>
+      <c r="F27">
         <v>1E-4</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>30</v>
       </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
       <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
         <v>0.99990000000000001</v>
       </c>
-      <c r="I27">
-        <v>0.999</v>
-      </c>
       <c r="J27">
+        <v>0.999</v>
+      </c>
+      <c r="K27">
         <v>9211</v>
       </c>
-      <c r="K27" s="3">
+      <c r="L27" s="3">
         <v>50000</v>
       </c>
-      <c r="L27">
+      <c r="M27">
         <v>1.469E-2</v>
       </c>
-      <c r="M27">
+      <c r="N27">
         <v>1.24E-2</v>
       </c>
-      <c r="N27" t="s">
+      <c r="O27" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>16</v>
       </c>
@@ -1593,38 +1738,41 @@
       <c r="D28">
         <v>32</v>
       </c>
-      <c r="E28">
+      <c r="E28" t="s">
+        <v>86</v>
+      </c>
+      <c r="F28">
         <v>1E-4</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>56</v>
       </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
       <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
         <v>0.99990000000000001</v>
       </c>
-      <c r="I28">
-        <v>0.999</v>
-      </c>
       <c r="J28">
+        <v>0.999</v>
+      </c>
+      <c r="K28">
         <v>9211</v>
       </c>
-      <c r="K28" s="3">
+      <c r="L28" s="3">
         <v>50000</v>
       </c>
-      <c r="L28">
+      <c r="M28">
         <v>6.4999999999999997E-3</v>
       </c>
-      <c r="M28">
+      <c r="N28">
         <v>6.6E-3</v>
       </c>
-      <c r="N28" t="s">
+      <c r="O28" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>17</v>
       </c>
@@ -1637,38 +1785,41 @@
       <c r="D29">
         <v>32</v>
       </c>
-      <c r="E29">
+      <c r="E29" t="s">
+        <v>86</v>
+      </c>
+      <c r="F29">
         <v>1E-4</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>30</v>
       </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
       <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
         <v>0.9</v>
       </c>
-      <c r="I29">
-        <v>0.999</v>
-      </c>
       <c r="J29">
+        <v>0.999</v>
+      </c>
+      <c r="K29">
         <v>9211</v>
       </c>
-      <c r="K29" s="3">
+      <c r="L29" s="3">
         <v>250000</v>
       </c>
-      <c r="L29">
+      <c r="M29">
         <v>1.9130000000000001E-2</v>
       </c>
-      <c r="M29">
+      <c r="N29">
         <v>1.6799999999999999E-2</v>
       </c>
-      <c r="N29" t="s">
+      <c r="O29" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>18</v>
       </c>
@@ -1681,38 +1832,41 @@
       <c r="D30">
         <v>32</v>
       </c>
-      <c r="E30">
+      <c r="E30" t="s">
+        <v>86</v>
+      </c>
+      <c r="F30">
         <v>1E-4</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>56</v>
       </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
       <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
         <v>0.99990000000000001</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <v>0.99</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <v>9211</v>
       </c>
-      <c r="K30" s="3">
+      <c r="L30" s="3">
         <v>50000</v>
       </c>
-      <c r="L30">
+      <c r="M30">
         <v>1.2E-2</v>
       </c>
-      <c r="M30">
+      <c r="N30">
         <v>8.3000000000000001E-3</v>
       </c>
-      <c r="N30" t="s">
+      <c r="O30" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>19</v>
       </c>
@@ -1725,50 +1879,53 @@
       <c r="D31">
         <v>32</v>
       </c>
-      <c r="E31">
+      <c r="E31" t="s">
+        <v>86</v>
+      </c>
+      <c r="F31">
         <v>1E-4</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>56</v>
       </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
       <c r="H31">
-        <v>0.99990000000000001</v>
+        <v>0</v>
       </c>
       <c r="I31">
         <v>0.99990000000000001</v>
       </c>
       <c r="J31">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="K31">
         <v>9211</v>
       </c>
-      <c r="K31" s="3">
+      <c r="L31" s="3">
         <v>50000</v>
       </c>
-      <c r="L31">
+      <c r="M31">
         <v>8.3400000000000002E-3</v>
       </c>
-      <c r="M31">
+      <c r="N31">
         <v>4.8999999999999998E-3</v>
       </c>
-      <c r="N31" t="s">
+      <c r="O31" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K32" s="3"/>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="K33" s="3"/>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L32" s="3"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L33" s="3"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>65</v>
       </c>
-      <c r="K34" s="3"/>
-    </row>
-    <row r="35" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="L34" s="3"/>
+    </row>
+    <row r="35" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>0</v>
       </c>
@@ -1779,46 +1936,49 @@
         <v>2</v>
       </c>
       <c r="E35" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F35" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="G35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H35" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="I35" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I35" s="1" t="s">
+      <c r="J35" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="J35" s="1" t="s">
+      <c r="K35" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K35" s="4" t="s">
+      <c r="L35" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L35" s="1" t="s">
+      <c r="M35" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M35" s="1" t="s">
+      <c r="N35" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N35" s="1" t="s">
+      <c r="O35" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="O35" s="1" t="s">
+      <c r="P35" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="P35" s="1" t="s">
+      <c r="Q35" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="Q35" s="1" t="s">
+      <c r="R35" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>20</v>
       </c>
@@ -1831,38 +1991,41 @@
       <c r="D36">
         <v>32</v>
       </c>
-      <c r="E36">
+      <c r="E36" t="s">
+        <v>86</v>
+      </c>
+      <c r="F36">
         <v>1E-4</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>56</v>
       </c>
-      <c r="G36">
-        <v>0</v>
-      </c>
       <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
         <v>0.99990000000000001</v>
       </c>
-      <c r="I36">
-        <v>0.999</v>
-      </c>
       <c r="J36">
+        <v>0.999</v>
+      </c>
+      <c r="K36">
         <v>9211</v>
       </c>
-      <c r="K36" s="3">
+      <c r="L36" s="3">
         <v>50000</v>
       </c>
-      <c r="L36">
+      <c r="M36">
         <v>9.9900000000000006E-3</v>
       </c>
-      <c r="M36">
+      <c r="N36">
         <v>6.4000000000000003E-3</v>
       </c>
-      <c r="Q36" t="s">
+      <c r="R36" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>21</v>
       </c>
@@ -1875,47 +2038,50 @@
       <c r="D37">
         <v>32</v>
       </c>
-      <c r="E37">
+      <c r="E37" t="s">
+        <v>86</v>
+      </c>
+      <c r="F37">
         <v>1E-4</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>56</v>
       </c>
-      <c r="G37">
-        <v>0</v>
-      </c>
       <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
         <v>0.99990000000000001</v>
       </c>
-      <c r="I37">
-        <v>0.999</v>
-      </c>
       <c r="J37">
+        <v>0.999</v>
+      </c>
+      <c r="K37">
         <v>9211</v>
       </c>
-      <c r="K37" s="3">
+      <c r="L37" s="3">
         <v>100000</v>
       </c>
-      <c r="L37">
+      <c r="M37">
         <v>5.4400000000000004E-3</v>
       </c>
-      <c r="M37">
+      <c r="N37">
         <v>3.8E-3</v>
       </c>
-      <c r="N37">
-        <v>1.7500000000000002E-2</v>
-      </c>
       <c r="O37">
-        <v>4.8999999999999998E-3</v>
+        <v>-1.7569619513137056</v>
       </c>
       <c r="P37">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="Q37" t="s">
+        <v>-2.3098039199714862</v>
+      </c>
+      <c r="Q37">
+        <v>-1.8239087409443189</v>
+      </c>
+      <c r="R37" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>22</v>
       </c>
@@ -1928,47 +2094,50 @@
       <c r="D38">
         <v>128</v>
       </c>
-      <c r="E38">
+      <c r="E38" t="s">
+        <v>86</v>
+      </c>
+      <c r="F38">
         <v>1E-4</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>56</v>
       </c>
-      <c r="G38">
-        <v>0</v>
-      </c>
       <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
         <v>0.99990000000000001</v>
       </c>
-      <c r="I38">
-        <v>0.999</v>
-      </c>
       <c r="J38">
+        <v>0.999</v>
+      </c>
+      <c r="K38">
         <v>9211</v>
       </c>
-      <c r="K38" s="3">
+      <c r="L38" s="3">
         <v>50000</v>
       </c>
-      <c r="L38">
+      <c r="M38">
         <v>4.4400000000000004E-3</v>
       </c>
-      <c r="M38">
+      <c r="N38">
         <v>2.8999999999999998E-3</v>
       </c>
-      <c r="N38">
-        <v>1.55E-2</v>
-      </c>
       <c r="O38">
-        <v>4.3E-3</v>
+        <v>-1.8096683018297086</v>
       </c>
       <c r="P38">
-        <v>1.129E-2</v>
-      </c>
-      <c r="Q38" t="s">
+        <v>-2.3665315444204134</v>
+      </c>
+      <c r="Q38">
+        <v>-1.9473060580750321</v>
+      </c>
+      <c r="R38" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>23</v>
       </c>
@@ -1981,47 +2150,50 @@
       <c r="D39">
         <v>256</v>
       </c>
-      <c r="E39">
+      <c r="E39" t="s">
+        <v>86</v>
+      </c>
+      <c r="F39">
         <v>1E-4</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>56</v>
       </c>
-      <c r="G39">
-        <v>0</v>
-      </c>
       <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
         <v>0.99990000000000001</v>
       </c>
-      <c r="I39">
-        <v>0.999</v>
-      </c>
       <c r="J39">
+        <v>0.999</v>
+      </c>
+      <c r="K39">
         <v>9211</v>
       </c>
-      <c r="K39" s="3">
+      <c r="L39" s="3">
         <v>50000</v>
       </c>
-      <c r="L39">
+      <c r="M39">
         <v>3.8449999999999999E-3</v>
       </c>
-      <c r="M39">
+      <c r="N39">
         <v>2.2000000000000001E-3</v>
       </c>
-      <c r="N39">
-        <v>1.3480000000000001E-2</v>
-      </c>
       <c r="O39">
-        <v>3.336E-3</v>
+        <v>-1.870310107800699</v>
       </c>
       <c r="P39">
-        <v>1.0149999999999999E-2</v>
-      </c>
-      <c r="Q39" t="s">
+        <v>-2.4767739580342991</v>
+      </c>
+      <c r="Q39">
+        <v>-1.9935339577507682</v>
+      </c>
+      <c r="R39" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>24</v>
       </c>
@@ -2034,47 +2206,50 @@
       <c r="D40">
         <v>128</v>
       </c>
-      <c r="E40">
+      <c r="E40" t="s">
+        <v>86</v>
+      </c>
+      <c r="F40">
         <v>1E-3</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>56</v>
       </c>
-      <c r="G40">
-        <v>0</v>
-      </c>
       <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
         <v>0.99990000000000001</v>
       </c>
-      <c r="I40">
-        <v>0.999</v>
-      </c>
       <c r="J40">
+        <v>0.999</v>
+      </c>
+      <c r="K40">
         <v>9211</v>
       </c>
-      <c r="K40" s="3">
+      <c r="L40" s="3">
         <v>50000</v>
       </c>
-      <c r="L40" s="5">
+      <c r="M40" s="5">
         <v>1.0430000000000001E-3</v>
       </c>
-      <c r="M40" s="6">
+      <c r="N40" s="6">
         <v>9.3528999999999997E-4</v>
       </c>
-      <c r="N40">
-        <v>3.7716009999999999E-3</v>
-      </c>
       <c r="O40">
-        <v>1.087382E-3</v>
+        <v>-2.4234742577862045</v>
       </c>
       <c r="P40">
-        <v>2.3932962000000001E-3</v>
-      </c>
-      <c r="Q40" t="s">
+        <v>-2.9636178603773242</v>
+      </c>
+      <c r="Q40">
+        <v>-2.6210035487476415</v>
+      </c>
+      <c r="R40" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>25</v>
       </c>
@@ -2087,47 +2262,50 @@
       <c r="D41">
         <v>32</v>
       </c>
-      <c r="E41">
+      <c r="E41" t="s">
+        <v>86</v>
+      </c>
+      <c r="F41">
         <v>1E-3</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>56</v>
       </c>
-      <c r="G41">
-        <v>0</v>
-      </c>
       <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
         <v>0.99990000000000001</v>
       </c>
-      <c r="I41">
-        <v>0.999</v>
-      </c>
       <c r="J41">
+        <v>0.999</v>
+      </c>
+      <c r="K41">
         <v>9211</v>
       </c>
-      <c r="K41" s="3">
+      <c r="L41" s="3">
         <v>50000</v>
       </c>
-      <c r="L41">
+      <c r="M41">
         <v>7.5900000000000004E-3</v>
       </c>
-      <c r="M41">
+      <c r="N41">
         <v>6.7000000000000002E-3</v>
       </c>
-      <c r="N41">
-        <v>2.6599999999999999E-2</v>
-      </c>
       <c r="O41">
-        <v>8.1499999999999993E-3</v>
+        <v>-1.575118363368933</v>
       </c>
       <c r="P41">
-        <v>1.83E-2</v>
-      </c>
-      <c r="Q41" t="s">
+        <v>-2.0888423912600236</v>
+      </c>
+      <c r="Q41">
+        <v>-1.7375489102695705</v>
+      </c>
+      <c r="R41" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>26</v>
       </c>
@@ -2140,47 +2318,50 @@
       <c r="D42">
         <v>32</v>
       </c>
-      <c r="E42">
+      <c r="E42" t="s">
+        <v>86</v>
+      </c>
+      <c r="F42">
         <v>0.01</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>56</v>
       </c>
-      <c r="G42">
-        <v>0</v>
-      </c>
       <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
         <v>0.99990000000000001</v>
       </c>
-      <c r="I42">
-        <v>0.999</v>
-      </c>
       <c r="J42">
+        <v>0.999</v>
+      </c>
+      <c r="K42">
         <v>9211</v>
       </c>
-      <c r="K42" s="3">
+      <c r="L42" s="3">
         <v>50000</v>
       </c>
-      <c r="L42" s="5">
+      <c r="M42" s="5">
         <v>5.0200000000000002E-3</v>
       </c>
-      <c r="M42" s="5">
+      <c r="N42" s="5">
         <v>3.8E-3</v>
       </c>
-      <c r="N42" s="5">
-        <v>1.7690000000000001E-2</v>
-      </c>
       <c r="O42" s="5">
-        <v>4.4169999999999999E-3</v>
+        <v>-1.7522721670902768</v>
       </c>
       <c r="P42" s="5">
-        <v>1.278E-2</v>
-      </c>
-      <c r="Q42" t="s">
+        <v>-2.3548726007416088</v>
+      </c>
+      <c r="Q42" s="5">
+        <v>-1.8934691461776187</v>
+      </c>
+      <c r="R42" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>27</v>
       </c>
@@ -2193,47 +2374,50 @@
       <c r="D43">
         <v>32</v>
       </c>
-      <c r="E43">
+      <c r="E43" t="s">
+        <v>86</v>
+      </c>
+      <c r="F43">
         <v>0.1</v>
       </c>
-      <c r="F43" t="s">
+      <c r="G43" t="s">
         <v>56</v>
       </c>
-      <c r="G43">
-        <v>0</v>
-      </c>
       <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
         <v>0.99990000000000001</v>
       </c>
-      <c r="I43">
-        <v>0.999</v>
-      </c>
       <c r="J43">
+        <v>0.999</v>
+      </c>
+      <c r="K43">
         <v>9211</v>
       </c>
-      <c r="K43" s="3">
+      <c r="L43" s="3">
         <v>50000</v>
       </c>
-      <c r="L43" s="5">
+      <c r="M43" s="5">
         <v>2.47E-2</v>
       </c>
-      <c r="M43" s="5">
+      <c r="N43" s="5">
         <v>1.8700000000000001E-2</v>
       </c>
-      <c r="N43" s="5">
-        <v>7.4200000000000002E-2</v>
-      </c>
       <c r="O43" s="5">
-        <v>3.3700000000000001E-2</v>
+        <v>-1.1295960947209729</v>
       </c>
       <c r="P43" s="5">
-        <v>6.5799999999999997E-2</v>
-      </c>
-      <c r="Q43" t="s">
+        <v>-1.4723700991286615</v>
+      </c>
+      <c r="Q43" s="5">
+        <v>-1.1817741063860445</v>
+      </c>
+      <c r="R43" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>28</v>
       </c>
@@ -2246,246 +2430,929 @@
       <c r="D44">
         <v>128</v>
       </c>
-      <c r="E44">
+      <c r="E44" t="s">
+        <v>86</v>
+      </c>
+      <c r="F44">
         <v>1E-3</v>
       </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>56</v>
       </c>
-      <c r="G44">
-        <v>0</v>
-      </c>
       <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
         <v>0.99990000000000001</v>
       </c>
-      <c r="I44">
-        <v>0.999</v>
-      </c>
       <c r="J44">
+        <v>0.999</v>
+      </c>
+      <c r="K44">
         <v>9211</v>
       </c>
-      <c r="K44" s="3">
+      <c r="L44" s="3">
+        <v>500000</v>
+      </c>
+      <c r="M44" s="5">
+        <v>5.9400000000000002E-4</v>
+      </c>
+      <c r="N44" s="6">
+        <v>4.8935000000000005E-4</v>
+      </c>
+      <c r="O44">
+        <v>-2.7019064678961024</v>
+      </c>
+      <c r="P44">
+        <v>-3.1678647412424379</v>
+      </c>
+      <c r="Q44">
+        <v>-2.8413157365100044</v>
+      </c>
+      <c r="R44" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>29</v>
+      </c>
+      <c r="B45" t="s">
+        <v>88</v>
+      </c>
+      <c r="C45">
+        <v>4</v>
+      </c>
+      <c r="D45">
+        <v>32</v>
+      </c>
+      <c r="E45" t="s">
+        <v>87</v>
+      </c>
+      <c r="F45">
+        <v>1E-3</v>
+      </c>
+      <c r="G45" t="s">
+        <v>56</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="J45">
+        <v>0.999</v>
+      </c>
+      <c r="K45">
+        <v>9211</v>
+      </c>
+      <c r="L45" s="3">
+        <v>5000</v>
+      </c>
+      <c r="M45" s="5">
+        <v>5.16E-2</v>
+      </c>
+      <c r="N45" s="5">
+        <v>4.4499999999999998E-2</v>
+      </c>
+      <c r="O45" s="5">
+        <v>-0.83268266525182388</v>
+      </c>
+      <c r="P45" s="5">
+        <v>-1.3467874862246563</v>
+      </c>
+      <c r="Q45" s="5">
+        <v>-0.8096683018297085</v>
+      </c>
+      <c r="R45" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>30</v>
+      </c>
+      <c r="B46" t="s">
+        <v>90</v>
+      </c>
+      <c r="C46">
+        <v>4</v>
+      </c>
+      <c r="D46">
+        <v>32</v>
+      </c>
+      <c r="E46" t="s">
+        <v>87</v>
+      </c>
+      <c r="F46">
+        <v>1E-3</v>
+      </c>
+      <c r="G46" t="s">
+        <v>56</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="J46">
+        <v>0.999</v>
+      </c>
+      <c r="K46">
+        <v>9211</v>
+      </c>
+      <c r="L46" s="8">
         <v>50000</v>
       </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="K45" s="3"/>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+      <c r="M46" s="5">
+        <v>1.1299999999999999E-2</v>
+      </c>
+      <c r="N46" s="5">
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="O46" s="5">
+        <v>-1.4133464648445535</v>
+      </c>
+      <c r="P46">
+        <v>-1.9079585501956591</v>
+      </c>
+      <c r="Q46">
+        <v>-1.5553208945901469</v>
+      </c>
+      <c r="R46" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>31</v>
+      </c>
+      <c r="B47" t="s">
+        <v>91</v>
+      </c>
+      <c r="C47">
+        <v>8</v>
+      </c>
+      <c r="D47">
+        <v>128</v>
+      </c>
+      <c r="E47" t="s">
+        <v>87</v>
+      </c>
+      <c r="F47">
+        <v>1E-3</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="J47">
+        <v>0.999</v>
+      </c>
+      <c r="K47">
+        <v>9211</v>
+      </c>
+      <c r="L47" s="8">
+        <v>50000</v>
+      </c>
+      <c r="M47">
+        <v>2.0867767999999999E-4</v>
+      </c>
+      <c r="N47" s="6">
+        <v>1.4396E-4</v>
+      </c>
+      <c r="O47">
+        <v>-3.1526804034467397</v>
+      </c>
+      <c r="P47">
+        <v>-3.6398908656159028</v>
+      </c>
+      <c r="Q47">
+        <v>-3.2835009750470601</v>
+      </c>
+      <c r="R47" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="K46" s="3"/>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="L49" s="3"/>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>36</v>
       </c>
-      <c r="K47" s="3"/>
-    </row>
-    <row r="48" spans="1:17" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C48" s="1" t="s">
+      <c r="L50" s="3"/>
+    </row>
+    <row r="51" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="E51" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F51" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F48" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G48" s="1" t="s">
+      <c r="G51" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H51" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H48" s="1" t="s">
+      <c r="I51" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I48" s="1" t="s">
+      <c r="J51" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="J48" s="1" t="s">
+      <c r="K51" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K48" s="4" t="s">
+      <c r="L51" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L48" s="1" t="s">
+      <c r="M51" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M48" s="1" t="s">
+      <c r="N51" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N48" s="1" t="s">
+      <c r="O51" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A52">
         <v>1</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B52" t="s">
         <v>41</v>
       </c>
-      <c r="K49" s="3"/>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A50">
+      <c r="L52" s="3"/>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A53">
         <v>2</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B53" t="s">
         <v>11</v>
       </c>
-      <c r="C50">
-        <v>4</v>
-      </c>
-      <c r="D50">
+      <c r="C53">
+        <v>4</v>
+      </c>
+      <c r="D53">
         <v>32</v>
       </c>
-      <c r="E50">
+      <c r="E53" t="s">
+        <v>86</v>
+      </c>
+      <c r="F53">
         <v>1E-4</v>
       </c>
-      <c r="F50">
-        <v>0</v>
-      </c>
-      <c r="G50">
-        <v>0</v>
-      </c>
-      <c r="H50">
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+      <c r="I53">
         <v>0.9</v>
       </c>
-      <c r="I50">
-        <v>0.999</v>
-      </c>
-      <c r="J50">
+      <c r="J53">
+        <v>0.999</v>
+      </c>
+      <c r="K53">
         <v>4310530</v>
       </c>
-      <c r="K50" s="3">
+      <c r="L53" s="3">
         <v>2000</v>
       </c>
-      <c r="L50">
+      <c r="M53">
         <v>5.0880000000000002E-2</v>
       </c>
-      <c r="M50">
+      <c r="N53">
         <v>5.5100000000000003E-2</v>
       </c>
-      <c r="N50" t="s">
+      <c r="O53" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A51">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A54">
         <v>3</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B54" t="s">
         <v>40</v>
       </c>
-      <c r="C51">
-        <v>4</v>
-      </c>
-      <c r="D51">
+      <c r="C54">
+        <v>4</v>
+      </c>
+      <c r="D54">
         <v>32</v>
       </c>
-      <c r="E51">
+      <c r="E54" t="s">
+        <v>86</v>
+      </c>
+      <c r="F54">
         <v>1E-4</v>
       </c>
-      <c r="F51">
-        <v>0</v>
-      </c>
-      <c r="G51">
-        <v>0</v>
-      </c>
-      <c r="H51">
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54">
         <v>0.9</v>
       </c>
-      <c r="I51">
-        <v>0.999</v>
-      </c>
-      <c r="J51">
+      <c r="J54">
+        <v>0.999</v>
+      </c>
+      <c r="K54">
         <v>4310530</v>
       </c>
-      <c r="K51" s="3">
+      <c r="L54" s="3">
         <v>12000</v>
       </c>
-      <c r="L51">
+      <c r="M54">
         <v>4.6289999999999998E-2</v>
       </c>
-      <c r="M51">
+      <c r="N54">
         <v>5.21E-2</v>
       </c>
-      <c r="N51" t="s">
+      <c r="O54" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-      <c r="K52" s="3"/>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K53" s="3"/>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K54" s="3"/>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K55" s="3"/>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K56" s="3"/>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K57" s="3"/>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K58" s="3"/>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K59" s="3"/>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K60" s="3"/>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K61" s="3"/>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K62" s="3"/>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K63" s="3"/>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K64" s="3"/>
-    </row>
-    <row r="65" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K65" s="3"/>
-    </row>
-    <row r="66" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K66" s="3"/>
-    </row>
-    <row r="67" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K67" s="3"/>
-    </row>
-    <row r="68" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K68" s="3"/>
-    </row>
-    <row r="69" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K69" s="3"/>
-    </row>
-    <row r="70" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K70" s="3"/>
-    </row>
-    <row r="71" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K71" s="3"/>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L55" s="3"/>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L59" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N59" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O59" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="P59" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q59" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="R59" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>4</v>
+      </c>
+      <c r="B60" t="s">
+        <v>11</v>
+      </c>
+      <c r="C60">
+        <v>7</v>
+      </c>
+      <c r="D60" s="1">
+        <v>64</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F60" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H60" s="1">
+        <v>0</v>
+      </c>
+      <c r="I60">
+        <v>0.99950000000000006</v>
+      </c>
+      <c r="J60">
+        <v>0.999</v>
+      </c>
+      <c r="K60" t="s">
+        <v>99</v>
+      </c>
+      <c r="L60" s="3">
+        <v>10000</v>
+      </c>
+      <c r="R60" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>5</v>
+      </c>
+      <c r="B61" t="s">
+        <v>96</v>
+      </c>
+      <c r="C61">
+        <v>9</v>
+      </c>
+      <c r="D61">
+        <v>64</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F61" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H61" s="1">
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <v>0.99950000000000006</v>
+      </c>
+      <c r="J61">
+        <v>0.999</v>
+      </c>
+      <c r="K61" t="s">
+        <v>99</v>
+      </c>
+      <c r="L61" s="3">
+        <v>10000</v>
+      </c>
+      <c r="R61" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>6</v>
+      </c>
+      <c r="B62" t="s">
+        <v>96</v>
+      </c>
+      <c r="C62">
+        <v>9</v>
+      </c>
+      <c r="D62">
+        <v>128</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F62" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H62" s="1">
+        <v>0</v>
+      </c>
+      <c r="I62">
+        <v>0.99950000000000006</v>
+      </c>
+      <c r="J62">
+        <v>0.999</v>
+      </c>
+      <c r="K62" t="s">
+        <v>99</v>
+      </c>
+      <c r="L62" s="3">
+        <v>10000</v>
+      </c>
+      <c r="M62" s="5">
+        <v>0.15898799999999999</v>
+      </c>
+      <c r="N62" s="5">
+        <v>0.1777</v>
+      </c>
+      <c r="O62">
+        <v>6.8185861746161619E-2</v>
+      </c>
+      <c r="P62">
+        <v>-1.4089353929735009</v>
+      </c>
+      <c r="Q62">
+        <v>-5.8985756294430272E-2</v>
+      </c>
+      <c r="R62" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>7</v>
+      </c>
+      <c r="B63" t="s">
+        <v>98</v>
+      </c>
+      <c r="C63">
+        <v>9</v>
+      </c>
+      <c r="D63">
+        <v>128</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F63" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H63" s="1">
+        <v>0</v>
+      </c>
+      <c r="I63">
+        <v>0.99950000000000006</v>
+      </c>
+      <c r="J63">
+        <v>0.999</v>
+      </c>
+      <c r="K63" t="s">
+        <v>99</v>
+      </c>
+      <c r="L63" s="3">
+        <v>20000</v>
+      </c>
+      <c r="M63" s="5">
+        <v>0.15448700000000001</v>
+      </c>
+      <c r="N63" s="5">
+        <v>0.1777</v>
+      </c>
+      <c r="O63" s="5">
+        <v>2.9383777685209667E-2</v>
+      </c>
+      <c r="P63" s="5">
+        <v>-1.4089353929735009</v>
+      </c>
+      <c r="Q63" s="5">
+        <v>-6.0980223551333534E-2</v>
+      </c>
+      <c r="R63" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>8</v>
+      </c>
+      <c r="B64" t="s">
+        <v>100</v>
+      </c>
+      <c r="C64">
+        <v>7</v>
+      </c>
+      <c r="D64">
+        <v>64</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F64" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="H64" s="1">
+        <v>0</v>
+      </c>
+      <c r="I64">
+        <v>0.99950000000000006</v>
+      </c>
+      <c r="J64">
+        <v>0.999</v>
+      </c>
+      <c r="K64" t="s">
+        <v>99</v>
+      </c>
+      <c r="L64" s="3">
+        <v>10000</v>
+      </c>
+      <c r="M64" s="5">
+        <v>0.178892</v>
+      </c>
+      <c r="N64" s="5">
+        <v>0.2341</v>
+      </c>
+      <c r="O64" s="5">
+        <v>-0.21724080737600285</v>
+      </c>
+      <c r="P64" s="5">
+        <v>-1.3010299956639813</v>
+      </c>
+      <c r="Q64" s="5">
+        <v>0.18127177155946156</v>
+      </c>
+      <c r="R64" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L65" s="3"/>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>105</v>
+      </c>
+      <c r="L66" s="3"/>
+    </row>
+    <row r="67" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="B67" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J67" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K67" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L67" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M67" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N67" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O67" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="P67" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q67" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="R67" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>9</v>
+      </c>
+      <c r="B68" t="s">
+        <v>11</v>
+      </c>
+      <c r="C68">
+        <v>6</v>
+      </c>
+      <c r="D68" s="1">
+        <v>64</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F68" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="G68" s="1">
+        <v>0</v>
+      </c>
+      <c r="H68" s="1">
+        <v>0</v>
+      </c>
+      <c r="I68">
+        <v>0.99950000000000006</v>
+      </c>
+      <c r="J68">
+        <v>0.999</v>
+      </c>
+      <c r="K68" t="s">
+        <v>99</v>
+      </c>
+      <c r="L68" s="3">
+        <v>10000</v>
+      </c>
+      <c r="M68" s="5">
+        <v>0.12509999999999999</v>
+      </c>
+      <c r="N68" s="5">
+        <v>0.1472</v>
+      </c>
+      <c r="O68" s="5">
+        <v>-0.43597000000000002</v>
+      </c>
+      <c r="P68" s="5">
+        <v>-1.7370000000000001</v>
+      </c>
+      <c r="Q68" s="5">
+        <v>-4.7999999999999996E-3</v>
+      </c>
+      <c r="R68" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>10</v>
+      </c>
+      <c r="B69" t="s">
+        <v>108</v>
+      </c>
+      <c r="C69">
+        <v>6</v>
+      </c>
+      <c r="D69">
+        <v>64</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F69">
+        <v>1E-3</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+      <c r="I69">
+        <v>0.99950000000000006</v>
+      </c>
+      <c r="J69">
+        <v>0.999</v>
+      </c>
+      <c r="K69" t="s">
+        <v>99</v>
+      </c>
+      <c r="L69" s="3">
+        <v>50000</v>
+      </c>
+      <c r="M69" s="5">
+        <v>4.5400000000000003E-2</v>
+      </c>
+      <c r="N69" s="5">
+        <v>9.9000000000000008E-3</v>
+      </c>
+      <c r="O69" s="5">
+        <v>-1.0045550000000001</v>
+      </c>
+      <c r="P69" s="5">
+        <v>-1.7515099999999999</v>
+      </c>
+      <c r="Q69" s="5">
+        <v>-0.49958000000000002</v>
+      </c>
+      <c r="R69" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>11</v>
+      </c>
+      <c r="B70" t="s">
+        <v>110</v>
+      </c>
+      <c r="C70">
+        <v>8</v>
+      </c>
+      <c r="D70">
+        <v>128</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F70">
+        <v>1E-3</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+      <c r="I70">
+        <v>0.99950000000000006</v>
+      </c>
+      <c r="J70">
+        <v>0.999</v>
+      </c>
+      <c r="K70" t="s">
+        <v>99</v>
+      </c>
+      <c r="L70" s="3">
+        <v>50000</v>
+      </c>
+      <c r="M70" s="5">
+        <v>3.1579999999999997E-2</v>
+      </c>
+      <c r="N70" s="5">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="O70" s="5">
+        <v>-1.1329400000000001</v>
+      </c>
+      <c r="P70" s="5">
+        <v>-1.7444999999999999</v>
+      </c>
+      <c r="Q70" s="5">
+        <v>-0.68230000000000002</v>
+      </c>
+      <c r="R70" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L71" s="3"/>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L72" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>